<commit_message>
correction on balance report
</commit_message>
<xml_diff>
--- a/uploads/excel_format/testbulkupload.xlsx
+++ b/uploads/excel_format/testbulkupload.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="83">
   <si>
     <t>cus_id</t>
   </si>
@@ -58,9 +58,6 @@
   </si>
   <si>
     <t>guarantor_occupation</t>
-  </si>
-  <si>
-    <t>guarantor_income</t>
   </si>
   <si>
     <t>residential type</t>
@@ -635,10 +632,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BK29"/>
+  <dimension ref="A1:BJ29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -658,55 +655,54 @@
     <col min="14" max="14" width="13.85546875" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="20.5703125" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="20.5703125" customWidth="1"/>
-    <col min="17" max="17" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="10" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="4.42578125" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="9" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="10" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="11" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="20.5703125" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="12" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="16.28515625" customWidth="1"/>
-    <col min="40" max="40" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="11" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="44" max="47" width="15.42578125" customWidth="1"/>
-    <col min="48" max="48" width="20.7109375" customWidth="1"/>
-    <col min="49" max="49" width="25.5703125" customWidth="1"/>
-    <col min="50" max="50" width="19.28515625" customWidth="1"/>
-    <col min="51" max="51" width="16.140625" customWidth="1"/>
-    <col min="52" max="52" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="13.5703125" customWidth="1"/>
-    <col min="54" max="54" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="55" max="55" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="56" max="56" width="12" bestFit="1" customWidth="1"/>
-    <col min="57" max="57" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="58" max="58" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="59" max="59" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="60" max="60" width="12" bestFit="1" customWidth="1"/>
-    <col min="61" max="61" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="62" max="62" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="63" max="63" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="10" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="4.42578125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="9" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="10" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="11" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="12" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="16.28515625" customWidth="1"/>
+    <col min="39" max="39" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="11" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="43" max="46" width="15.42578125" customWidth="1"/>
+    <col min="47" max="47" width="20.7109375" customWidth="1"/>
+    <col min="48" max="48" width="25.5703125" customWidth="1"/>
+    <col min="49" max="49" width="19.28515625" customWidth="1"/>
+    <col min="50" max="50" width="16.140625" customWidth="1"/>
+    <col min="51" max="51" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="13.5703125" customWidth="1"/>
+    <col min="53" max="53" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="12" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="12" bestFit="1" customWidth="1"/>
+    <col min="60" max="60" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="61" max="61" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="62" max="62" width="11.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:63" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:62" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B1" s="6" t="s">
         <v>0</v>
@@ -751,7 +747,7 @@
         <v>13</v>
       </c>
       <c r="P1" s="6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="Q1" s="6" t="s">
         <v>14</v>
@@ -811,10 +807,10 @@
         <v>32</v>
       </c>
       <c r="AJ1" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="AK1" s="6" t="s">
         <v>33</v>
-      </c>
-      <c r="AK1" s="6" t="s">
-        <v>79</v>
       </c>
       <c r="AL1" s="6" t="s">
         <v>34</v>
@@ -832,10 +828,10 @@
         <v>38</v>
       </c>
       <c r="AQ1" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="AR1" s="6" t="s">
         <v>39</v>
-      </c>
-      <c r="AR1" s="6" t="s">
-        <v>73</v>
       </c>
       <c r="AS1" s="6" t="s">
         <v>40</v>
@@ -844,10 +840,10 @@
         <v>41</v>
       </c>
       <c r="AU1" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="AV1" s="6" t="s">
         <v>42</v>
-      </c>
-      <c r="AV1" s="6" t="s">
-        <v>65</v>
       </c>
       <c r="AW1" s="6" t="s">
         <v>43</v>
@@ -859,10 +855,10 @@
         <v>45</v>
       </c>
       <c r="AZ1" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="BA1" s="6" t="s">
         <v>46</v>
-      </c>
-      <c r="BA1" s="6" t="s">
-        <v>66</v>
       </c>
       <c r="BB1" s="6" t="s">
         <v>47</v>
@@ -891,11 +887,8 @@
       <c r="BJ1" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="BK1" s="6" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="2" spans="1:63" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:62" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -903,10 +896,10 @@
         <v>332209876544</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E2" s="5">
         <v>37233</v>
@@ -918,13 +911,13 @@
         <v>9876512342</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="L2" s="4">
         <v>890989089096</v>
@@ -936,226 +929,226 @@
         <v>76</v>
       </c>
       <c r="O2" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="P2" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="Q2" s="3" t="s">
         <v>70</v>
-      </c>
-      <c r="P2" s="3" t="s">
-        <v>64</v>
       </c>
       <c r="R2" s="3" t="s">
         <v>71</v>
       </c>
       <c r="S2" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="T2" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="U2" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="Y2" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="Z2" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="AB2" s="3">
+        <v>890000</v>
+      </c>
+      <c r="AC2" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="Z2" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="AA2" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="AC2" s="3">
-        <v>890000</v>
-      </c>
       <c r="AD2" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="AE2" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="AF2" s="3">
+        <v>74</v>
+      </c>
+      <c r="AE2" s="3">
         <v>76000</v>
       </c>
-      <c r="AG2" s="3" t="s">
-        <v>67</v>
+      <c r="AF2" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="AJ2" s="3" t="s">
+        <v>76</v>
       </c>
       <c r="AK2" s="3" t="s">
         <v>77</v>
       </c>
       <c r="AL2" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="AM2" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="AM2" s="3">
+        <v>12</v>
+      </c>
+      <c r="AN2" s="3">
+        <v>5</v>
+      </c>
+      <c r="AO2" s="3">
+        <v>1</v>
+      </c>
+      <c r="AP2" s="3">
+        <v>2</v>
+      </c>
+      <c r="AQ2" s="3">
+        <v>450000</v>
+      </c>
+      <c r="AR2" s="3">
+        <v>890000</v>
+      </c>
+      <c r="AS2" s="3">
+        <v>908000</v>
+      </c>
+      <c r="AT2" s="3">
+        <v>786</v>
+      </c>
+      <c r="AU2" s="3">
+        <v>450</v>
+      </c>
+      <c r="AV2" s="3">
+        <v>567</v>
+      </c>
+      <c r="AW2" s="3">
+        <v>98000</v>
+      </c>
+      <c r="AX2" s="5">
+        <v>45484</v>
+      </c>
+      <c r="AY2" s="5">
+        <v>45485</v>
+      </c>
+      <c r="AZ2" s="5">
+        <v>37481</v>
+      </c>
+      <c r="BA2" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="BD2" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="BE2" s="3">
+        <v>890000</v>
+      </c>
+      <c r="BF2" s="4">
+        <v>98787678676897</v>
+      </c>
+      <c r="BG2" s="3">
+        <v>32456566766</v>
+      </c>
+      <c r="BH2" s="5">
+        <v>45572</v>
+      </c>
+      <c r="BI2" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="BJ2" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="AN2" s="3">
-        <v>12</v>
-      </c>
-      <c r="AO2" s="3">
-        <v>5</v>
-      </c>
-      <c r="AP2" s="3">
-        <v>1</v>
-      </c>
-      <c r="AQ2" s="3">
-        <v>2</v>
-      </c>
-      <c r="AR2" s="3">
-        <v>450000</v>
-      </c>
-      <c r="AS2" s="3">
-        <v>890000</v>
-      </c>
-      <c r="AT2" s="3">
-        <v>908000</v>
-      </c>
-      <c r="AU2" s="3">
-        <v>786</v>
-      </c>
-      <c r="AV2" s="3">
-        <v>450</v>
-      </c>
-      <c r="AW2" s="3">
-        <v>567</v>
-      </c>
-      <c r="AX2" s="3">
-        <v>98000</v>
-      </c>
-      <c r="AY2" s="5">
-        <v>45484</v>
-      </c>
-      <c r="AZ2" s="5">
-        <v>45485</v>
-      </c>
-      <c r="BA2" s="5">
-        <v>37481</v>
-      </c>
-      <c r="BB2" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="BE2" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="BF2" s="3">
-        <v>890000</v>
-      </c>
-      <c r="BG2" s="4">
-        <v>98787678676897</v>
-      </c>
-      <c r="BH2" s="3">
-        <v>32456566766</v>
-      </c>
-      <c r="BI2" s="5">
-        <v>45572</v>
-      </c>
-      <c r="BJ2" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="BK2" s="3" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="3" spans="1:63" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:62" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
       <c r="E3" s="2"/>
       <c r="L3" s="1"/>
+      <c r="AX3" s="2"/>
       <c r="AY3" s="2"/>
       <c r="AZ3" s="2"/>
-      <c r="BA3" s="2"/>
-      <c r="BI3" s="2"/>
-    </row>
-    <row r="4" spans="1:63" x14ac:dyDescent="0.25">
+      <c r="BH3" s="2"/>
+    </row>
+    <row r="4" spans="1:62" x14ac:dyDescent="0.25">
       <c r="B4" s="1"/>
       <c r="E4" s="2"/>
       <c r="L4" s="1"/>
+      <c r="AX4" s="2"/>
       <c r="AY4" s="2"/>
       <c r="AZ4" s="2"/>
-      <c r="BA4" s="2"/>
-      <c r="BI4" s="2"/>
-    </row>
-    <row r="5" spans="1:63" x14ac:dyDescent="0.25">
+      <c r="BH4" s="2"/>
+    </row>
+    <row r="5" spans="1:62" x14ac:dyDescent="0.25">
       <c r="B5" s="1"/>
       <c r="E5" s="2"/>
       <c r="L5" s="1"/>
+      <c r="AX5" s="2"/>
       <c r="AY5" s="2"/>
       <c r="AZ5" s="2"/>
-      <c r="BA5" s="2"/>
-      <c r="BG5" s="1"/>
-      <c r="BI5" s="2"/>
-    </row>
-    <row r="6" spans="1:63" x14ac:dyDescent="0.25">
+      <c r="BF5" s="1"/>
+      <c r="BH5" s="2"/>
+    </row>
+    <row r="6" spans="1:62" x14ac:dyDescent="0.25">
       <c r="B6" s="1"/>
       <c r="E6" s="2"/>
       <c r="L6" s="1"/>
+      <c r="AX6" s="2"/>
       <c r="AY6" s="2"/>
       <c r="AZ6" s="2"/>
-      <c r="BA6" s="2"/>
-      <c r="BG6" s="1"/>
-      <c r="BI6" s="2"/>
-    </row>
-    <row r="7" spans="1:63" x14ac:dyDescent="0.25">
+      <c r="BF6" s="1"/>
+      <c r="BH6" s="2"/>
+    </row>
+    <row r="7" spans="1:62" x14ac:dyDescent="0.25">
       <c r="B7" s="1"/>
       <c r="E7" s="2"/>
       <c r="L7" s="1"/>
+      <c r="AX7" s="2"/>
       <c r="AY7" s="2"/>
       <c r="AZ7" s="2"/>
-      <c r="BA7" s="2"/>
-      <c r="BG7" s="1"/>
-      <c r="BI7" s="2"/>
-    </row>
-    <row r="8" spans="1:63" x14ac:dyDescent="0.25">
+      <c r="BF7" s="1"/>
+      <c r="BH7" s="2"/>
+    </row>
+    <row r="8" spans="1:62" x14ac:dyDescent="0.25">
       <c r="B8" s="1"/>
       <c r="E8" s="2"/>
       <c r="L8" s="1"/>
+      <c r="AX8" s="2"/>
       <c r="AY8" s="2"/>
       <c r="AZ8" s="2"/>
-      <c r="BA8" s="2"/>
-      <c r="BG8" s="1"/>
-      <c r="BI8" s="2"/>
-    </row>
-    <row r="9" spans="1:63" x14ac:dyDescent="0.25">
+      <c r="BF8" s="1"/>
+      <c r="BH8" s="2"/>
+    </row>
+    <row r="9" spans="1:62" x14ac:dyDescent="0.25">
       <c r="B9" s="1"/>
       <c r="E9" s="2"/>
       <c r="L9" s="1"/>
+      <c r="AX9" s="2"/>
       <c r="AY9" s="2"/>
       <c r="AZ9" s="2"/>
-      <c r="BA9" s="2"/>
-      <c r="BG9" s="1"/>
-      <c r="BI9" s="2"/>
-    </row>
-    <row r="10" spans="1:63" x14ac:dyDescent="0.25">
+      <c r="BF9" s="1"/>
+      <c r="BH9" s="2"/>
+    </row>
+    <row r="10" spans="1:62" x14ac:dyDescent="0.25">
       <c r="B10" s="1"/>
       <c r="E10" s="2"/>
       <c r="L10" s="1"/>
+      <c r="AX10" s="2"/>
       <c r="AY10" s="2"/>
       <c r="AZ10" s="2"/>
-      <c r="BA10" s="2"/>
-      <c r="BG10" s="1"/>
-      <c r="BI10" s="2"/>
-    </row>
-    <row r="11" spans="1:63" x14ac:dyDescent="0.25">
+      <c r="BF10" s="1"/>
+      <c r="BH10" s="2"/>
+    </row>
+    <row r="11" spans="1:62" x14ac:dyDescent="0.25">
       <c r="B11" s="1"/>
       <c r="E11" s="2"/>
       <c r="L11" s="1"/>
+      <c r="AX11" s="2"/>
       <c r="AY11" s="2"/>
       <c r="AZ11" s="2"/>
-      <c r="BA11" s="2"/>
-      <c r="BI11" s="2"/>
-    </row>
-    <row r="12" spans="1:63" x14ac:dyDescent="0.25">
+      <c r="BH11" s="2"/>
+    </row>
+    <row r="12" spans="1:62" x14ac:dyDescent="0.25">
       <c r="B12" s="1"/>
       <c r="E12" s="2"/>
       <c r="L12" s="1"/>
+      <c r="AX12" s="2"/>
       <c r="AY12" s="2"/>
       <c r="AZ12" s="2"/>
-      <c r="BA12" s="2"/>
-      <c r="BI12" s="2"/>
-    </row>
-    <row r="13" spans="1:63" x14ac:dyDescent="0.25">
+      <c r="BH12" s="2"/>
+    </row>
+    <row r="13" spans="1:62" x14ac:dyDescent="0.25">
       <c r="B13" s="1"/>
     </row>
-    <row r="14" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:62" x14ac:dyDescent="0.25">
       <c r="B14" s="1"/>
     </row>
-    <row r="15" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:62" x14ac:dyDescent="0.25">
       <c r="B15" s="1"/>
     </row>
-    <row r="16" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:62" x14ac:dyDescent="0.25">
       <c r="B16" s="1"/>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.25">

</xml_diff>